<commit_message>
Added a package to the Requirements.txt -> openpxl
</commit_message>
<xml_diff>
--- a/Output/todays_ufc_event.xlsx
+++ b/Output/todays_ufc_event.xlsx
@@ -456,12 +456,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>Alexander</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Oliveira</t>
+          <t>Volkov</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -474,16 +474,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Justin</t>
+          <t>Jairzinho</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Gaethje</t>
+          <t>Rozenstruik</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -492,16 +492,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Carla</t>
+          <t>Dan</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Esparza</t>
+          <t>Ige</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -510,16 +510,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rose</t>
+          <t>Movsar</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Namajunas</t>
+          <t>Evloev</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -533,11 +533,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Chandler</t>
+          <t>Trizano</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -546,16 +546,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tony</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ferguson</t>
+          <t>Almeida</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -564,12 +564,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ovince</t>
+          <t>Karine</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Saint Preux</t>
+          <t>Silva</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -582,16 +582,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mauricio</t>
+          <t>Poliana</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Rua</t>
+          <t>Botelho</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -600,12 +600,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Randy</t>
+          <t>Ode</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Brown</t>
+          <t>Osbourne</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -618,12 +618,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Khaos</t>
+          <t>Zarrukh</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Adashev</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -636,12 +636,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Francisco</t>
+          <t>Alonzo</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Trinaldo</t>
+          <t>Menifield</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -654,16 +654,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Danny</t>
+          <t>Askar</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Roberts</t>
+          <t>Mozharov</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -672,12 +672,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Macy</t>
+          <t>Felice</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Chiasson</t>
+          <t>Herrig</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -690,12 +690,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Norma</t>
+          <t>Karolina</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Dumont</t>
+          <t>Kowalkiewicz</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -708,12 +708,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Brandon</t>
+          <t>Joe</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Royval</t>
+          <t>Solecki</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -726,12 +726,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Matt</t>
+          <t>Alex</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Schnell</t>
+          <t>Da Silva</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -744,12 +744,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Blagoy</t>
+          <t>Damon</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Ivanov</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -762,12 +762,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Marcos</t>
+          <t>Dan</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Rogerio de Lima</t>
+          <t>Argueta</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -780,12 +780,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Andre</t>
+          <t>Niklas</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Fialho</t>
+          <t>Stolze</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -798,12 +798,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cameron</t>
+          <t>Benoit</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>VanCamp</t>
+          <t>Saint Denis</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -816,12 +816,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Tracy</t>
+          <t>Johnny</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Cortez</t>
+          <t>Munoz</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -834,16 +834,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Melissa</t>
+          <t>Tony</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Gatto</t>
+          <t>Gravely</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -852,16 +852,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>CJ</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Vergara</t>
+          <t>Molina</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -870,12 +870,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Kleydson</t>
+          <t>Zhalgas</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Rodrigues</t>
+          <t>Zhumagulov</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -888,12 +888,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Loopy</t>
+          <t>Rinat</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Godinez</t>
+          <t>Fakhretdinov</t>
         </is>
       </c>
       <c r="D26" t="n">
@@ -906,12 +906,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ariane</t>
+          <t>Andreas</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Carnelossi</t>
+          <t>Michailidis</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -924,16 +924,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Journey</t>
+          <t>Erin</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Newson</t>
+          <t>Blanchfield</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -942,12 +942,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fernie</t>
+          <t>JJ</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>Aldrich</t>
         </is>
       </c>
       <c r="D29" t="n">

</xml_diff>

<commit_message>
Changed location of the input CSV for easier access to it.
</commit_message>
<xml_diff>
--- a/Output/todays_ufc_event.xlsx
+++ b/Output/todays_ufc_event.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>Cory</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Volkov</t>
+          <t>Sandhagen</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -474,12 +474,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jairzinho</t>
+          <t>Rob</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Rozenstruik</t>
+          <t>Font</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -492,12 +492,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Jessica</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ige</t>
+          <t>Andrade</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -510,16 +510,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Movsar</t>
+          <t>Tatiana</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Evloev</t>
+          <t>Suarez</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -528,16 +528,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Dustin</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Trizano</t>
+          <t>Jacoby</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -546,16 +546,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Kennedy</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Almeida</t>
+          <t>Nzechukwu</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -564,16 +564,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Karine</t>
+          <t>Diego</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Silva</t>
+          <t>Lopes</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -582,12 +582,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Poliana</t>
+          <t>Gavin</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Botelho</t>
+          <t>Tucker</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -600,12 +600,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ode</t>
+          <t>Tanner</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Osbourne</t>
+          <t>Boser</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -618,16 +618,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Zarrukh</t>
+          <t>Aleksa</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Adashev</t>
+          <t>Camur</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -636,12 +636,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Alonzo</t>
+          <t>Ignacio</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Menifield</t>
+          <t>Bahamondes</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -654,12 +654,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Askar</t>
+          <t>Ludovit</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Mozharov</t>
+          <t>Klein</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -672,12 +672,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Felice</t>
+          <t>Kyler</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Herrig</t>
+          <t>Phillips</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -690,12 +690,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Karolina</t>
+          <t>Raoni</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Kowalkiewicz</t>
+          <t>Barcelos</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -708,16 +708,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Jeremiah</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Solecki</t>
+          <t>Wells</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -726,12 +726,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>Carlston</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Da Silva</t>
+          <t>Harris</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -744,12 +744,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Damon</t>
+          <t>Billy</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Quarantillo</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -762,12 +762,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Damon</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Argueta</t>
+          <t>Jackson</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -780,12 +780,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Niklas</t>
+          <t>Cody</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Stolze</t>
+          <t>Durden</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -798,12 +798,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Benoit</t>
+          <t>Jake</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Saint Denis</t>
+          <t>Hadley</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -816,16 +816,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Johnny</t>
+          <t>Sean</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Munoz</t>
+          <t>Woodson</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -834,12 +834,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Tony</t>
+          <t>Dennis</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Gravely</t>
+          <t>Buzukja</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -852,12 +852,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Ode</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Molina</t>
+          <t>Osbourne</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -870,87 +870,15 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Zhalgas</t>
+          <t>Assu</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Zhumagulov</t>
+          <t>Almabayev</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Rinat</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Fakhretdinov</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Andreas</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Michailidis</t>
-        </is>
-      </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Erin</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Blanchfield</t>
-        </is>
-      </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>JJ</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Aldrich</t>
-        </is>
-      </c>
-      <c r="D29" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Created a new directory for input -> Dataset now is in the input folder with the script pulling from it
</commit_message>
<xml_diff>
--- a/Output/todays_ufc_event.xlsx
+++ b/Output/todays_ufc_event.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,12 +456,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cory</t>
+          <t>Brendan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sandhagen</t>
+          <t>Allen</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -474,12 +474,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rob</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Font</t>
+          <t>Craig</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -492,16 +492,16 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jessica</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Andrade</t>
+          <t>Morales</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -510,12 +510,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Tatiana</t>
+          <t>Jake</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Suarez</t>
+          <t>Matthews</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -528,16 +528,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dustin</t>
+          <t>Chase</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jacoby</t>
+          <t>Hooper</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -546,16 +546,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kennedy</t>
+          <t>Jordan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Nzechukwu</t>
+          <t>Leavitt</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -564,12 +564,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Payton</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Lopes</t>
+          <t>Talbott</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -582,16 +582,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Gavin</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Tucker</t>
+          <t>Aguirre</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -600,12 +600,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Tanner</t>
+          <t>Amanda</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Boser</t>
+          <t>Ribas</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -618,16 +618,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Aleksa</t>
+          <t>Luana</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Camur</t>
+          <t>Pinheiro</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -636,16 +636,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ignacio</t>
+          <t>Myktybek</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Bahamondes</t>
+          <t>Orolbai</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -654,12 +654,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ludovit</t>
+          <t>Uros</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Klein</t>
+          <t>Medic</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -672,12 +672,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kyler</t>
+          <t>Joanderson</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Phillips</t>
+          <t>Brito</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -690,12 +690,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Raoni</t>
+          <t>Jonathan</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Barcelos</t>
+          <t>Pearce</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -708,16 +708,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Jeremiah</t>
+          <t>Jose</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Wells</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -726,12 +726,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Carlston</t>
+          <t>Chad</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Harris</t>
+          <t>Anheliger</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -744,16 +744,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Billy</t>
+          <t>Christian</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Quarantillo</t>
+          <t>Leroy Duncan</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -762,16 +762,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Damon</t>
+          <t>Denis</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Jackson</t>
+          <t>Tiuliulin</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -780,12 +780,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cody</t>
+          <t>Mick</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Durden</t>
+          <t>Parkin</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -798,12 +798,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jake</t>
+          <t>Caio</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Hadley</t>
+          <t>Machado</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -816,12 +816,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sean</t>
+          <t>Jeka</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Woodson</t>
+          <t>Saragih</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -834,12 +834,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Dennis</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Buzukja</t>
+          <t>Alexander</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -852,12 +852,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Ode</t>
+          <t>Ailin</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Osbourne</t>
+          <t>Perez</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -870,16 +870,52 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Assu</t>
+          <t>Lucie</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Almabayev</t>
+          <t>Pudilova</t>
         </is>
       </c>
       <c r="D25" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Trey</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Ogden</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Nikolas</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Motta</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>